<commit_message>
Updating for pos integration
</commit_message>
<xml_diff>
--- a/Data/Tables/targets.xlsx
+++ b/Data/Tables/targets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quirozmoreno.1/Documents/GitHub/apple_phytochemicals/Data/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED6D734-27A5-894C-A7E3-1842ECB79EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727DDB31-D8D3-3B44-B457-B2848B3511C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="700" windowWidth="27040" windowHeight="15360" activeTab="3" xr2:uid="{65E5DED9-F2BA-E545-8C0E-73D75F3592BA}"/>
+    <workbookView xWindow="1600" yWindow="760" windowWidth="27040" windowHeight="15360" activeTab="2" xr2:uid="{65E5DED9-F2BA-E545-8C0E-73D75F3592BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Pos" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="170">
   <si>
     <t>3-Hydroxybenzaldehyde</t>
   </si>
@@ -873,6 +873,27 @@
   <si>
     <t>(+)-Catechin</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>trans</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>-3-coumaric acid</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -882,7 +903,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="33">
+  <fonts count="35">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1078,6 +1099,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1169,7 +1203,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="32" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1337,8 +1371,7 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1797,7 +1830,7 @@
         <v>134.07316489999999</v>
       </c>
       <c r="C4" s="6">
-        <f t="shared" ref="C3:C66" si="2">B4+1.0072</f>
+        <f t="shared" ref="C4:C66" si="2">B4+1.0072</f>
         <v>135.08036490000001</v>
       </c>
       <c r="D4" s="6">
@@ -4146,7 +4179,7 @@
         <v>484.07723920000001</v>
       </c>
       <c r="C68" s="6">
-        <f t="shared" ref="C67:C70" si="9">B68+1.0072</f>
+        <f t="shared" ref="C68:C70" si="9">B68+1.0072</f>
         <v>485.08443920000002</v>
       </c>
       <c r="D68" s="6">
@@ -4396,7 +4429,7 @@
         <v>135.08036490000001</v>
       </c>
       <c r="D4" s="6">
-        <f t="shared" ref="D3:D66" si="2">B4-1.0072</f>
+        <f t="shared" ref="D4:D66" si="2">B4-1.0072</f>
         <v>133.06596489999998</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -6890,7 +6923,7 @@
         <v>485.08443920000002</v>
       </c>
       <c r="D68" s="6">
-        <f t="shared" ref="D67:D70" si="23">B68-1.0072</f>
+        <f t="shared" ref="D68:D70" si="23">B68-1.0072</f>
         <v>483.0700392</v>
       </c>
       <c r="E68" s="3" t="s">
@@ -6998,16 +7031,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C5B812-0665-B14A-BB3A-0C3879E743C8}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="33.1640625" style="83" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="10.83203125" style="83"/>
+    <col min="2" max="8" width="10.83203125" style="83"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -7038,27 +7071,25 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="83" t="s">
-        <v>9</v>
+        <v>169</v>
       </c>
       <c r="B2" s="83">
-        <v>155.03390869999998</v>
+        <v>165.05464000000001</v>
       </c>
       <c r="C2" s="83">
         <v>10</v>
       </c>
-      <c r="D2" s="84">
-        <v>1.84</v>
+      <c r="D2" s="83">
+        <v>177</v>
       </c>
       <c r="E2" s="83">
-        <f>D2-0.06</f>
-        <v>1.78</v>
+        <v>176</v>
       </c>
       <c r="F2" s="83">
-        <f>D2+0.06</f>
-        <v>1.9000000000000001</v>
+        <v>181</v>
       </c>
       <c r="G2" s="83" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H2" s="83">
         <v>1000</v>
@@ -7066,24 +7097,24 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="83" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B3" s="83">
-        <v>165.05463999999998</v>
+        <v>303.01356720000001</v>
       </c>
       <c r="C3" s="83">
         <v>10</v>
       </c>
-      <c r="D3" s="84">
-        <v>2.9129999999999998</v>
+      <c r="D3" s="83">
+        <v>2.8420000000000001</v>
       </c>
       <c r="E3" s="83">
-        <f t="shared" ref="E3:E22" si="0">D3-0.06</f>
-        <v>2.8529999999999998</v>
+        <f t="shared" ref="E3:E19" si="0">D3-0.06</f>
+        <v>2.782</v>
       </c>
       <c r="F3" s="83">
-        <f t="shared" ref="F3:F22" si="1">D3+0.06</f>
-        <v>2.9729999999999999</v>
+        <f t="shared" ref="F3:F19" si="1">D3+0.06</f>
+        <v>2.9020000000000001</v>
       </c>
       <c r="G3" s="83" t="s">
         <v>162</v>
@@ -7094,27 +7125,25 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="83" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B4" s="83">
-        <v>303.01356720000001</v>
+        <v>303.04989999999998</v>
       </c>
       <c r="C4" s="83">
         <v>10</v>
       </c>
-      <c r="D4" s="84">
-        <v>2.8420000000000001</v>
+      <c r="D4" s="83">
+        <v>216</v>
       </c>
       <c r="E4" s="83">
-        <f t="shared" si="0"/>
-        <v>2.782</v>
+        <v>213</v>
       </c>
       <c r="F4" s="83">
-        <f t="shared" si="1"/>
-        <v>2.9020000000000001</v>
+        <v>222</v>
       </c>
       <c r="G4" s="83" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H4" s="83">
         <v>1000</v>
@@ -7122,27 +7151,25 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="83" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="83">
-        <v>303.04989999999998</v>
+        <v>355.10237999999998</v>
       </c>
       <c r="C5" s="83">
         <v>10</v>
       </c>
-      <c r="D5" s="84">
-        <v>3.6019999999999999</v>
+      <c r="D5" s="83">
+        <v>134</v>
       </c>
       <c r="E5" s="83">
-        <f t="shared" si="0"/>
-        <v>3.5419999999999998</v>
+        <v>130</v>
       </c>
       <c r="F5" s="83">
-        <f t="shared" si="1"/>
-        <v>3.6619999999999999</v>
+        <v>140</v>
       </c>
       <c r="G5" s="83" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H5" s="83">
         <v>1000</v>
@@ -7150,27 +7177,25 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="83" t="s">
-        <v>25</v>
+        <v>164</v>
       </c>
       <c r="B6" s="83">
-        <v>355.10237999999998</v>
+        <v>596.17349999999999</v>
       </c>
       <c r="C6" s="83">
         <v>10</v>
       </c>
-      <c r="D6" s="84">
-        <v>2.552</v>
+      <c r="D6" s="83">
+        <v>135</v>
       </c>
       <c r="E6" s="83">
-        <f t="shared" si="0"/>
-        <v>2.492</v>
+        <v>131</v>
       </c>
       <c r="F6" s="83">
-        <f t="shared" si="1"/>
-        <v>2.6120000000000001</v>
+        <v>140</v>
       </c>
       <c r="G6" s="83" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H6" s="83">
         <v>1000</v>
@@ -7178,24 +7203,24 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="83" t="s">
-        <v>164</v>
+        <v>27</v>
       </c>
       <c r="B7" s="83">
-        <v>596.17349999999999</v>
+        <v>611.16067999999996</v>
       </c>
       <c r="C7" s="83">
         <v>10</v>
       </c>
-      <c r="D7" s="84">
-        <v>2.2799999999999998</v>
+      <c r="D7" s="83">
+        <v>2.7839999999999998</v>
       </c>
       <c r="E7" s="83">
         <f t="shared" si="0"/>
-        <v>2.2199999999999998</v>
+        <v>2.7239999999999998</v>
       </c>
       <c r="F7" s="83">
         <f t="shared" si="1"/>
-        <v>2.34</v>
+        <v>2.8439999999999999</v>
       </c>
       <c r="G7" s="83" t="s">
         <v>162</v>
@@ -7206,27 +7231,25 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="83" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B8" s="83">
-        <v>611.16067999999996</v>
+        <v>291.08632999999998</v>
       </c>
       <c r="C8" s="83">
         <v>10</v>
       </c>
-      <c r="D8" s="84">
-        <v>2.7839999999999998</v>
+      <c r="D8" s="83">
+        <v>148</v>
       </c>
       <c r="E8" s="83">
-        <f t="shared" si="0"/>
-        <v>2.7239999999999998</v>
+        <v>144</v>
       </c>
       <c r="F8" s="83">
-        <f t="shared" si="1"/>
-        <v>2.8439999999999999</v>
+        <v>152</v>
       </c>
       <c r="G8" s="83" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H8" s="83">
         <v>1000</v>
@@ -7234,27 +7257,25 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="83" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B9" s="83">
-        <v>291.08632999999998</v>
+        <v>437.14423999999997</v>
       </c>
       <c r="C9" s="83">
         <v>10</v>
       </c>
-      <c r="D9" s="84">
-        <v>2.3889999999999998</v>
+      <c r="D9" s="83">
+        <v>191</v>
       </c>
       <c r="E9" s="83">
-        <f t="shared" si="0"/>
-        <v>2.3289999999999997</v>
+        <v>189</v>
       </c>
       <c r="F9" s="83">
-        <f t="shared" si="1"/>
-        <v>2.4489999999999998</v>
+        <v>195</v>
       </c>
       <c r="G9" s="83" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H9" s="83">
         <v>1000</v>
@@ -7262,27 +7283,25 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="83" t="s">
-        <v>34</v>
+        <v>163</v>
       </c>
       <c r="B10" s="83">
-        <v>303.04994999999997</v>
+        <v>449.10785999999996</v>
       </c>
       <c r="C10" s="83">
         <v>10</v>
       </c>
-      <c r="D10" s="84">
-        <v>3.4489999999999998</v>
+      <c r="D10" s="83">
+        <v>182</v>
       </c>
       <c r="E10" s="83">
-        <f t="shared" si="0"/>
-        <v>3.3889999999999998</v>
+        <v>179</v>
       </c>
       <c r="F10" s="83">
-        <f t="shared" si="1"/>
-        <v>3.5089999999999999</v>
+        <v>186</v>
       </c>
       <c r="G10" s="83" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H10" s="83">
         <v>1000</v>
@@ -7290,24 +7309,24 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="83" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B11" s="83">
-        <v>437.14423999999997</v>
+        <v>449.10785999999996</v>
       </c>
       <c r="C11" s="83">
         <v>10</v>
       </c>
-      <c r="D11" s="84">
-        <v>3.1419999999999999</v>
+      <c r="D11" s="83">
+        <v>3.0331999999999999</v>
       </c>
       <c r="E11" s="83">
         <f t="shared" si="0"/>
-        <v>3.0819999999999999</v>
+        <v>2.9731999999999998</v>
       </c>
       <c r="F11" s="83">
         <f t="shared" si="1"/>
-        <v>3.202</v>
+        <v>3.0931999999999999</v>
       </c>
       <c r="G11" s="83" t="s">
         <v>162</v>
@@ -7318,27 +7337,25 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="83" t="s">
-        <v>163</v>
+        <v>41</v>
       </c>
       <c r="B12" s="83">
-        <v>449.10785999999996</v>
+        <v>465.10276999999996</v>
       </c>
       <c r="C12" s="83">
         <v>10</v>
       </c>
-      <c r="D12" s="84">
-        <v>3.0129999999999999</v>
+      <c r="D12" s="83">
+        <v>169</v>
       </c>
       <c r="E12" s="83">
-        <f t="shared" si="0"/>
-        <v>2.9529999999999998</v>
+        <v>165</v>
       </c>
       <c r="F12" s="83">
-        <f t="shared" si="1"/>
-        <v>3.073</v>
+        <v>175</v>
       </c>
       <c r="G12" s="83" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H12" s="83">
         <v>1000</v>
@@ -7346,27 +7363,25 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="83" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B13" s="83">
-        <v>449.10785999999996</v>
+        <v>473.36250000000001</v>
       </c>
       <c r="C13" s="83">
         <v>10</v>
       </c>
-      <c r="D13" s="84">
-        <v>3.0331999999999999</v>
+      <c r="D13" s="83">
+        <v>408</v>
       </c>
       <c r="E13" s="83">
-        <f t="shared" si="0"/>
-        <v>2.9731999999999998</v>
+        <v>405</v>
       </c>
       <c r="F13" s="83">
-        <f t="shared" si="1"/>
-        <v>3.0931999999999999</v>
+        <v>411</v>
       </c>
       <c r="G13" s="83" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H13" s="83">
         <v>1000</v>
@@ -7374,27 +7389,25 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="83" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B14" s="83">
-        <v>465.10276999999996</v>
+        <v>579.14969999999994</v>
       </c>
       <c r="C14" s="83">
         <v>10</v>
       </c>
-      <c r="D14" s="84">
-        <v>2.863</v>
+      <c r="D14" s="83">
+        <v>126</v>
       </c>
       <c r="E14" s="83">
-        <f t="shared" si="0"/>
-        <v>2.8029999999999999</v>
+        <v>123</v>
       </c>
       <c r="F14" s="83">
-        <f t="shared" si="1"/>
-        <v>2.923</v>
+        <v>131</v>
       </c>
       <c r="G14" s="83" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H14" s="83">
         <v>1000</v>
@@ -7402,27 +7415,25 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="83" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B15" s="83">
-        <v>473.36250000000001</v>
+        <v>579.14969999999994</v>
       </c>
       <c r="C15" s="83">
         <v>10</v>
       </c>
-      <c r="D15" s="84">
-        <v>6.7569999999999997</v>
+      <c r="D15" s="83">
+        <v>140</v>
       </c>
       <c r="E15" s="83">
-        <f t="shared" si="0"/>
-        <v>6.6970000000000001</v>
+        <v>137</v>
       </c>
       <c r="F15" s="83">
-        <f t="shared" si="1"/>
-        <v>6.8169999999999993</v>
+        <v>145</v>
       </c>
       <c r="G15" s="83" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H15" s="83">
         <v>1000</v>
@@ -7430,27 +7441,25 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="83" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B16" s="83">
-        <v>577.13406999999995</v>
+        <v>625.17629999999997</v>
       </c>
       <c r="C16" s="83">
         <v>10</v>
       </c>
-      <c r="D16" s="84">
-        <v>2.8719999999999999</v>
+      <c r="D16" s="83">
+        <v>178</v>
       </c>
       <c r="E16" s="83">
-        <f t="shared" si="0"/>
-        <v>2.8119999999999998</v>
+        <v>175</v>
       </c>
       <c r="F16" s="83">
-        <f t="shared" si="1"/>
-        <v>2.9319999999999999</v>
+        <v>182</v>
       </c>
       <c r="G16" s="83" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H16" s="83">
         <v>1000</v>
@@ -7458,27 +7467,25 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="83" t="s">
-        <v>47</v>
+        <v>118</v>
       </c>
       <c r="B17" s="83">
-        <v>579.14969999999994</v>
+        <v>867.21309999999994</v>
       </c>
       <c r="C17" s="83">
-        <v>10</v>
-      </c>
-      <c r="D17" s="84">
-        <v>2.097</v>
+        <v>15</v>
+      </c>
+      <c r="D17" s="83">
+        <v>149</v>
       </c>
       <c r="E17" s="83">
-        <f t="shared" si="0"/>
-        <v>2.0369999999999999</v>
+        <v>146</v>
       </c>
       <c r="F17" s="83">
-        <f t="shared" si="1"/>
-        <v>2.157</v>
+        <v>155</v>
       </c>
       <c r="G17" s="83" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H17" s="83">
         <v>1000</v>
@@ -7486,27 +7493,25 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="83" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B18" s="83">
-        <v>579.14969999999994</v>
+        <v>183.08629999999999</v>
       </c>
       <c r="C18" s="83">
         <v>10</v>
       </c>
-      <c r="D18" s="84">
-        <v>2.33</v>
+      <c r="D18" s="83">
+        <v>20</v>
       </c>
       <c r="E18" s="83">
-        <f t="shared" si="0"/>
-        <v>2.27</v>
+        <v>18</v>
       </c>
       <c r="F18" s="83">
-        <f t="shared" si="1"/>
-        <v>2.39</v>
+        <v>22</v>
       </c>
       <c r="G18" s="83" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H18" s="83">
         <v>1000</v>
@@ -7514,113 +7519,27 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="83" t="s">
-        <v>55</v>
+        <v>168</v>
       </c>
       <c r="B19" s="83">
-        <v>625.17629999999997</v>
+        <v>291.08632999999998</v>
       </c>
       <c r="C19" s="83">
         <v>10</v>
       </c>
-      <c r="D19" s="84">
-        <v>2.992</v>
+      <c r="D19" s="83">
+        <v>135</v>
       </c>
       <c r="E19" s="83">
-        <f t="shared" si="0"/>
-        <v>2.9319999999999999</v>
+        <v>131</v>
       </c>
       <c r="F19" s="83">
-        <f t="shared" si="1"/>
-        <v>3.052</v>
+        <v>140</v>
       </c>
       <c r="G19" s="83" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H19" s="83">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="83" t="s">
-        <v>118</v>
-      </c>
-      <c r="B20" s="83">
-        <v>867.21309999999994</v>
-      </c>
-      <c r="C20" s="83">
-        <v>15</v>
-      </c>
-      <c r="D20" s="84">
-        <v>2.4889999999999999</v>
-      </c>
-      <c r="E20" s="83">
-        <f t="shared" si="0"/>
-        <v>2.4289999999999998</v>
-      </c>
-      <c r="F20" s="83">
-        <f t="shared" si="1"/>
-        <v>2.5489999999999999</v>
-      </c>
-      <c r="G20" s="83" t="s">
-        <v>162</v>
-      </c>
-      <c r="H20" s="83">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="83" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="83">
-        <v>183.08629999999999</v>
-      </c>
-      <c r="C21" s="83">
-        <v>10</v>
-      </c>
-      <c r="D21" s="84">
-        <v>0.35599999999999998</v>
-      </c>
-      <c r="E21" s="83">
-        <f t="shared" si="0"/>
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="F21" s="83">
-        <f t="shared" si="1"/>
-        <v>0.41599999999999998</v>
-      </c>
-      <c r="G21" s="83" t="s">
-        <v>162</v>
-      </c>
-      <c r="H21" s="83">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="83" t="s">
-        <v>63</v>
-      </c>
-      <c r="B22" s="83">
-        <v>291.08632999999998</v>
-      </c>
-      <c r="C22" s="83">
-        <v>10</v>
-      </c>
-      <c r="D22" s="84">
-        <v>2.2290000000000001</v>
-      </c>
-      <c r="E22" s="83">
-        <f t="shared" si="0"/>
-        <v>2.169</v>
-      </c>
-      <c r="F22" s="83">
-        <f t="shared" si="1"/>
-        <v>2.2890000000000001</v>
-      </c>
-      <c r="G22" s="83" t="s">
-        <v>162</v>
-      </c>
-      <c r="H22" s="83">
         <v>1000</v>
       </c>
     </row>
@@ -7633,7 +7552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF240FB-2FCE-3544-B6BE-26A9E3D416B5}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="168" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="168" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -7643,28 +7562,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="83" t="s">
+      <c r="A1" t="s">
         <v>154</v>
       </c>
-      <c r="B1" s="83" t="s">
+      <c r="B1" t="s">
         <v>155</v>
       </c>
-      <c r="C1" s="83" t="s">
+      <c r="C1" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="83" t="s">
+      <c r="D1" t="s">
         <v>157</v>
       </c>
-      <c r="E1" s="83" t="s">
+      <c r="E1" t="s">
         <v>158</v>
       </c>
-      <c r="F1" s="83" t="s">
+      <c r="F1" t="s">
         <v>159</v>
       </c>
-      <c r="G1" s="83" t="s">
+      <c r="G1" t="s">
         <v>160</v>
       </c>
-      <c r="H1" s="83" t="s">
+      <c r="H1" t="s">
         <v>161</v>
       </c>
     </row>

</xml_diff>